<commit_message>
Created simple views for apps and models for collections and users
</commit_message>
<xml_diff>
--- a/content/burndown.xlsx
+++ b/content/burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecad7fb2fd623e16/School/Appstate/2021Spring/Capstone/AppStateCapstone/content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Capstone\AppStateCapstone\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{2589019F-1D43-4464-B0F8-762BF3489693}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B5F5C7D5-91FC-E647-9794-7C64D6DE48AA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C387D8F-85E6-4BA0-A865-B90D0BFDF34D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="500" windowWidth="27380" windowHeight="17500" xr2:uid="{58AE2564-334E-0F42-91A8-57075DA461D6}"/>
+    <workbookView xWindow="8730" yWindow="2355" windowWidth="29220" windowHeight="17640" xr2:uid="{58AE2564-334E-0F42-91A8-57075DA461D6}"/>
   </bookViews>
   <sheets>
     <sheet name="EffortRawData" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{F54DA456-B0A3-C34F-B4EB-10A01303D66C}">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{F54DA456-B0A3-C34F-B4EB-10A01303D66C}">
       <text>
         <r>
           <rPr>
@@ -151,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{808B3ECB-8534-8340-B4A5-7738962116A3}">
+    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{808B3ECB-8534-8340-B4A5-7738962116A3}">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{F65F7D0D-B627-2142-AF9F-B9EAB8D18538}">
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{F65F7D0D-B627-2142-AF9F-B9EAB8D18538}">
       <text>
         <r>
           <rPr>
@@ -200,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{F8C402E0-4F70-FC48-80B3-01096083B0CC}">
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{F8C402E0-4F70-FC48-80B3-01096083B0CC}">
       <text>
         <r>
           <rPr>
@@ -224,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{1A1B4E01-05C7-BC4E-AA18-AAB726C802E1}">
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{1A1B4E01-05C7-BC4E-AA18-AAB726C802E1}">
       <text>
         <r>
           <rPr>
@@ -248,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{87FE40A0-93E0-8749-A5E3-6AAA55399195}">
+    <comment ref="G23" authorId="0" shapeId="0" xr:uid="{87FE40A0-93E0-8749-A5E3-6AAA55399195}">
       <text>
         <r>
           <rPr>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Project Name:</t>
   </si>
@@ -375,12 +375,6 @@
     <t>Admin Card Update Page Feature (Display update)</t>
   </si>
   <si>
-    <t>Login Page Bug (Bad Creds)</t>
-  </si>
-  <si>
-    <t>Login Page Bug (Layout)</t>
-  </si>
-  <si>
     <t>#2</t>
   </si>
   <si>
@@ -390,12 +384,6 @@
     <t>#4</t>
   </si>
   <si>
-    <t>#6</t>
-  </si>
-  <si>
-    <t>#7</t>
-  </si>
-  <si>
     <t>#9</t>
   </si>
   <si>
@@ -426,10 +414,19 @@
     <t>Lifecounter (will be split up)</t>
   </si>
   <si>
-    <t>Learn PHP</t>
-  </si>
-  <si>
     <t>Discussed switching to django</t>
+  </si>
+  <si>
+    <t>Setup local django env + 4 apps</t>
+  </si>
+  <si>
+    <t>Setup MySQL db instance</t>
+  </si>
+  <si>
+    <t>Create Login Page (django)</t>
+  </si>
+  <si>
+    <t>Learn django</t>
   </si>
 </sst>
 </file>
@@ -798,43 +795,43 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>127</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>121.5</c:v>
+                  <c:v>94.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>99.5</c:v>
+                  <c:v>66.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>94</c:v>
+                  <c:v>59.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88.5</c:v>
+                  <c:v>52.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>83</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77.5</c:v>
+                  <c:v>39.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>66.5</c:v>
+                  <c:v>25.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>61</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>55.5</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -927,43 +924,43 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>127</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>121.5</c:v>
+                  <c:v>94.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>105</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1056,40 +1053,40 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>127</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>116.41666666666667</c:v>
+                  <c:v>91.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>105.83333333333334</c:v>
+                  <c:v>83.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95.250000000000014</c:v>
+                  <c:v>75.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.666666666666686</c:v>
+                  <c:v>66.666666666666686</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74.083333333333357</c:v>
+                  <c:v>58.33333333333335</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>63.500000000000021</c:v>
+                  <c:v>50.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52.916666666666686</c:v>
+                  <c:v>41.666666666666679</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42.33333333333335</c:v>
+                  <c:v>33.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.750000000000014</c:v>
+                  <c:v>25.000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.166666666666679</c:v>
+                  <c:v>16.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.583333333333345</c:v>
+                  <c:v>8.3333333333333375</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -2202,22 +2199,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE15858-1152-CB4E-BE11-BC0471701F8D}">
-  <dimension ref="A1:R84"/>
+  <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.1640625" customWidth="1"/>
+    <col min="1" max="1" width="45.125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2237,7 +2234,7 @@
       <c r="L1" s="16"/>
       <c r="M1" s="16"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2248,7 +2245,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
@@ -2256,7 +2253,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2264,77 +2261,77 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="10">
-        <f>COUNTA(A7:A84)</f>
-        <v>17</v>
+        <f>COUNTA(A7:A81)</f>
+        <v>18</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="10">
-        <f>SUM(D7:D84)</f>
-        <v>127</v>
+        <f>SUM(D7:D81)</f>
+        <v>100</v>
       </c>
       <c r="E5" s="11">
-        <f>SUM(E7:E84)</f>
-        <v>22</v>
+        <f>SUM(E7:E81)</f>
+        <v>27</v>
       </c>
       <c r="F5" s="10">
-        <f>D5-SUM(F7:F84)</f>
-        <v>121.5</v>
+        <f>D5-SUM(F7:F81)</f>
+        <v>94.5</v>
       </c>
       <c r="G5" s="10">
-        <f>F5-SUM(G7:G84)</f>
-        <v>108</v>
+        <f>F5-SUM(G7:G81)</f>
+        <v>81</v>
       </c>
       <c r="H5" s="10">
-        <f>G5-SUM(H7:H84)</f>
-        <v>105</v>
+        <f>G5-SUM(H7:H81)</f>
+        <v>73</v>
       </c>
       <c r="I5" s="10">
-        <f>H5-SUM(I7:I84)</f>
-        <v>105</v>
+        <f>H5-SUM(I7:I81)</f>
+        <v>73</v>
       </c>
       <c r="J5" s="10">
-        <f>I5-SUM(J7:J84)</f>
-        <v>105</v>
+        <f>I5-SUM(J7:J81)</f>
+        <v>73</v>
       </c>
       <c r="K5" s="10">
-        <f>J5-SUM(K7:K84)</f>
-        <v>105</v>
+        <f>J5-SUM(K7:K81)</f>
+        <v>73</v>
       </c>
       <c r="L5" s="10">
-        <f>K5-SUM(L7:L84)</f>
-        <v>105</v>
+        <f>K5-SUM(L7:L81)</f>
+        <v>73</v>
       </c>
       <c r="M5" s="10">
-        <f>L5-SUM(M7:M84)</f>
-        <v>105</v>
+        <f>L5-SUM(M7:M81)</f>
+        <v>73</v>
       </c>
       <c r="N5" s="10">
-        <f>M5-SUM(N7:N84)</f>
-        <v>105</v>
+        <f>M5-SUM(N7:N81)</f>
+        <v>73</v>
       </c>
       <c r="O5" s="10">
-        <f>N5-SUM(O7:O84)</f>
-        <v>105</v>
+        <f>N5-SUM(O7:O81)</f>
+        <v>73</v>
       </c>
       <c r="P5" s="10">
-        <f>O5-SUM(P7:P84)</f>
-        <v>105</v>
+        <f>O5-SUM(P7:P81)</f>
+        <v>73</v>
       </c>
       <c r="Q5" s="10">
-        <f>P5-SUM(Q7:Q84)</f>
-        <v>105</v>
+        <f>P5-SUM(Q7:Q81)</f>
+        <v>73</v>
       </c>
       <c r="R5" s="10">
-        <f>Q5-SUM(R7:R84)</f>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+        <f>Q5-SUM(R7:R81)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2390,112 +2387,91 @@
         <v>44314</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="23">
-        <v>44233</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="24">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44238</v>
+      </c>
+      <c r="D7" s="2">
+        <v>15</v>
+      </c>
+      <c r="E7" s="6">
+        <f>SUM(F7:R7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44238</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <v>2</v>
       </c>
-      <c r="E7" s="25">
-        <f t="shared" ref="E7:E13" si="0">SUM(F7:R7)</f>
+      <c r="E8" s="6">
+        <f>SUM(F8:R8)</f>
         <v>2</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-    </row>
-    <row r="8" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="23">
-        <v>44233</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="24">
-        <v>4</v>
-      </c>
-      <c r="E8" s="25">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="F8" s="24">
-        <v>2.5</v>
-      </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-    </row>
-    <row r="9" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="23">
-        <v>44233</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="24">
-        <v>7</v>
-      </c>
-      <c r="E9" s="25">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24">
-        <v>7</v>
-      </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44238</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <f>SUM(F9:R9)</f>
+        <v>2</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1">
-        <v>44237</v>
+        <v>44238</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E10" s="6">
         <f>SUM(F10:R10)</f>
@@ -2514,29 +2490,16 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1">
-        <v>44233</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="2">
-        <v>10</v>
-      </c>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="6">
-        <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2">
-        <v>5.5</v>
-      </c>
+        <f>SUM(F11:R11)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -2548,26 +2511,28 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>44233</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D12" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E12:E14" si="0">SUM(F12:R12)</f>
+        <v>6.5</v>
+      </c>
+      <c r="F12" s="2">
         <v>1</v>
       </c>
-      <c r="F12" s="2"/>
       <c r="G12" s="2">
-        <v>1</v>
+        <v>5.5</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2580,25 +2545,27 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>44233</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E13" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -2610,21 +2577,21 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1">
         <v>44233</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" ref="E14:E65" si="1">SUM(F14:R14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14" s="2"/>
@@ -2640,21 +2607,21 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>44233</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E15:E62" si="1">SUM(F15:R15)</f>
         <v>0</v>
       </c>
       <c r="F15" s="2"/>
@@ -2670,15 +2637,15 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1">
         <v>44233</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2">
         <v>10</v>
@@ -2700,18 +2667,18 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>44233</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="1"/>
@@ -2730,18 +2697,18 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1">
         <v>44233</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" si="1"/>
@@ -2760,21 +2727,21 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1">
         <v>44233</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E19" s="6">
-        <f>SUM(F19:R19)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F19" s="2"/>
@@ -2790,21 +2757,19 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1">
-        <v>44233</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>44237</v>
+      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E20" s="6">
-        <f>SUM(F20:R20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F20" s="2"/>
@@ -2820,26 +2785,17 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="1">
-        <v>44237</v>
-      </c>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2">
-        <v>4</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
+      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -2850,17 +2806,10 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="1">
-        <v>44237</v>
-      </c>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2">
-        <v>30</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2878,121 +2827,163 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="1">
+    <row r="23" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="23">
+        <v>44233</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="24">
+        <v>2</v>
+      </c>
+      <c r="E23" s="25">
+        <f>SUM(F23:R23)</f>
+        <v>2</v>
+      </c>
+      <c r="F23" s="24">
+        <v>2</v>
+      </c>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+    </row>
+    <row r="24" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="23">
+        <v>44233</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="24">
+        <v>4</v>
+      </c>
+      <c r="E24" s="25">
+        <f>SUM(F24:R24)</f>
+        <v>2.5</v>
+      </c>
+      <c r="F24" s="24">
+        <v>2.5</v>
+      </c>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+    </row>
+    <row r="25" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="23">
+        <v>44233</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="24">
+        <v>7</v>
+      </c>
+      <c r="E25" s="25">
+        <f>SUM(F25:R25)</f>
+        <v>7</v>
+      </c>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24">
+        <v>7</v>
+      </c>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+    </row>
+    <row r="26" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="23">
         <v>44237</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2">
+      <c r="C26" s="24"/>
+      <c r="D26" s="24">
         <v>2</v>
       </c>
-      <c r="E23" s="6">
-        <f t="shared" si="1"/>
+      <c r="E26" s="25">
+        <f>SUM(F26:R26)</f>
         <v>2</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2">
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24">
         <v>2</v>
       </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+    </row>
+    <row r="27" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="23">
+        <v>44237</v>
+      </c>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24">
+        <v>2</v>
+      </c>
+      <c r="E27" s="25">
+        <f>SUM(F27:R27)</f>
+        <v>2</v>
+      </c>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24">
+        <v>2</v>
+      </c>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -3013,7 +3004,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -3034,7 +3025,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -3055,7 +3046,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -3076,7 +3067,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -3097,7 +3088,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -3118,7 +3109,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -3139,7 +3130,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -3160,7 +3151,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -3181,7 +3172,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -3202,7 +3193,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -3223,7 +3214,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -3244,7 +3235,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -3265,7 +3256,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -3286,7 +3277,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -3307,7 +3298,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -3328,7 +3319,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -3349,7 +3340,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -3370,7 +3361,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -3391,7 +3382,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -3412,7 +3403,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -3433,7 +3424,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -3454,7 +3445,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -3475,7 +3466,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -3496,7 +3487,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -3517,7 +3508,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -3538,7 +3529,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -3559,7 +3550,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -3580,7 +3571,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -3601,7 +3592,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -3622,7 +3613,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -3643,7 +3634,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -3664,7 +3655,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -3685,7 +3676,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -3706,7 +3697,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -3727,12 +3718,12 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E63:E81" si="2">SUM(F63:R63)</f>
         <v>0</v>
       </c>
       <c r="F63" s="2"/>
@@ -3748,12 +3739,12 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F64" s="2"/>
@@ -3769,12 +3760,12 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F65" s="2"/>
@@ -3790,12 +3781,12 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="6">
-        <f t="shared" ref="E66:E84" si="2">SUM(F66:R66)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F66" s="2"/>
@@ -3811,7 +3802,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -3832,7 +3823,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -3853,7 +3844,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -3874,7 +3865,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -3895,7 +3886,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -3916,7 +3907,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -3937,7 +3928,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -3958,7 +3949,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -3979,107 +3970,44 @@
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B75" s="1"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E75" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
-      <c r="K75" s="2"/>
-      <c r="L75" s="2"/>
-      <c r="M75" s="2"/>
-      <c r="N75" s="2"/>
-      <c r="O75" s="2"/>
-      <c r="P75" s="2"/>
-      <c r="Q75" s="2"/>
-    </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B76" s="1"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+    </row>
+    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E76" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
-      <c r="N76" s="2"/>
-      <c r="O76" s="2"/>
-      <c r="P76" s="2"/>
-      <c r="Q76" s="2"/>
-    </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B77" s="1"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+    </row>
+    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E77" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
-      <c r="K77" s="2"/>
-      <c r="L77" s="2"/>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
-      <c r="O77" s="2"/>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="2"/>
-    </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E78" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E79" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E80" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E81" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E82" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E83" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E84" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4100,7 +4028,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4115,9 +4043,9 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>12</v>
       </c>
@@ -4127,7 +4055,7 @@
       <c r="E2" s="26"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -4135,7 +4063,7 @@
       <c r="E3" s="26"/>
       <c r="F3" s="17"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
@@ -4143,7 +4071,7 @@
       <c r="E4" s="26"/>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
@@ -4151,11 +4079,11 @@
       <c r="E5" s="26"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F6" s="17"/>
       <c r="R6" s="13"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>15</v>
       </c>
@@ -4173,66 +4101,66 @@
       </c>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <f>EffortRawData!F$6</f>
         <v>44230</v>
       </c>
       <c r="B8" s="9">
         <f>EffortRawData!D5</f>
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="C8" s="9">
         <f>B8</f>
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="D8" s="9">
         <f>EffortRawData!D5</f>
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <f>EffortRawData!G$6</f>
         <v>44237</v>
       </c>
       <c r="B9" s="9">
         <f>EffortRawData!F5</f>
-        <v>121.5</v>
+        <v>94.5</v>
       </c>
       <c r="C9" s="9">
         <f>C8-(C$8/$E$19)</f>
-        <v>116.41666666666667</v>
+        <v>91.666666666666671</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" ref="D9:D10" si="0">IF($B9=$B8,MAX(0,$D8-($B$8-$D8)/$E8),$B9)</f>
-        <v>121.5</v>
+        <v>94.5</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <f>EffortRawData!H$6</f>
         <v>44244</v>
       </c>
       <c r="B10" s="9">
         <f>EffortRawData!G5</f>
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="C10" s="9">
         <f t="shared" ref="C10:C20" si="1">C9-(C$8/$E$19)</f>
-        <v>105.83333333333334</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="E10" s="2">
         <v>3</v>
@@ -4240,22 +4168,22 @@
       <c r="F10" s="18"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <f>EffortRawData!I$6</f>
         <v>44251</v>
       </c>
       <c r="B11" s="9">
         <f>EffortRawData!H5</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C11" s="9">
         <f t="shared" si="1"/>
-        <v>95.250000000000014</v>
+        <v>75.000000000000014</v>
       </c>
       <c r="D11" s="9">
         <f>IF($B11=$B10,MAX(0,$D10-($B$8-$D10)/$E10),$B11)</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="E11" s="2">
         <v>4</v>
@@ -4263,190 +4191,190 @@
       <c r="F11" s="19"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <f>EffortRawData!J$6</f>
         <v>44258</v>
       </c>
       <c r="B12" s="9">
         <f>EffortRawData!I5</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C12" s="9">
         <f t="shared" si="1"/>
-        <v>84.666666666666686</v>
+        <v>66.666666666666686</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" ref="D12:D20" si="2">IF($B12=$B11,MAX(0,$D11-($B$8-$D11)/$E11),$B12)</f>
-        <v>99.5</v>
+        <v>66.25</v>
       </c>
       <c r="E12" s="2">
         <v>5</v>
       </c>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <f>EffortRawData!K$6</f>
         <v>44265</v>
       </c>
       <c r="B13" s="9">
         <f>EffortRawData!J5</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C13" s="9">
         <f t="shared" si="1"/>
-        <v>74.083333333333357</v>
+        <v>58.33333333333335</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="2"/>
-        <v>94</v>
+        <v>59.5</v>
       </c>
       <c r="E13" s="2">
         <v>6</v>
       </c>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <f>EffortRawData!L$6</f>
         <v>44272</v>
       </c>
       <c r="B14" s="9">
         <f>EffortRawData!K5</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C14" s="9">
         <f t="shared" si="1"/>
-        <v>63.500000000000021</v>
+        <v>50.000000000000014</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="2"/>
-        <v>88.5</v>
+        <v>52.75</v>
       </c>
       <c r="E14" s="2">
         <v>7</v>
       </c>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <f>EffortRawData!M$6</f>
         <v>44279</v>
       </c>
       <c r="B15" s="9">
         <f>EffortRawData!L5</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C15" s="9">
         <f t="shared" si="1"/>
-        <v>52.916666666666686</v>
+        <v>41.666666666666679</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="2"/>
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="E15" s="2">
         <v>8</v>
       </c>
       <c r="F15" s="18"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <f>EffortRawData!N$6</f>
         <v>44286</v>
       </c>
       <c r="B16" s="9">
         <f>EffortRawData!M5</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C16" s="9">
         <f t="shared" si="1"/>
-        <v>42.33333333333335</v>
+        <v>33.333333333333343</v>
       </c>
       <c r="D16" s="9">
         <f t="shared" si="2"/>
-        <v>77.5</v>
+        <v>39.25</v>
       </c>
       <c r="E16" s="2">
         <v>9</v>
       </c>
       <c r="F16" s="18"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <f>EffortRawData!O$6</f>
         <v>44293</v>
       </c>
       <c r="B17" s="9">
         <f>EffortRawData!N5</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C17" s="9">
         <f t="shared" si="1"/>
-        <v>31.750000000000014</v>
+        <v>25.000000000000007</v>
       </c>
       <c r="D17" s="9">
         <f t="shared" si="2"/>
-        <v>72</v>
+        <v>32.5</v>
       </c>
       <c r="E17" s="2">
         <v>10</v>
       </c>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <f>EffortRawData!P$6</f>
         <v>44300</v>
       </c>
       <c r="B18" s="9">
         <f>EffortRawData!O5</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C18" s="9">
         <f t="shared" si="1"/>
-        <v>21.166666666666679</v>
+        <v>16.666666666666671</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" si="2"/>
-        <v>66.5</v>
+        <v>25.75</v>
       </c>
       <c r="E18" s="2">
         <v>11</v>
       </c>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <f>EffortRawData!Q$6</f>
         <v>44307</v>
       </c>
       <c r="B19" s="9">
         <f>EffortRawData!P5</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C19" s="9">
         <f t="shared" si="1"/>
-        <v>10.583333333333345</v>
+        <v>8.3333333333333375</v>
       </c>
       <c r="D19" s="9">
         <f t="shared" si="2"/>
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="E19" s="2">
         <v>12</v>
       </c>
       <c r="F19" s="18"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <f>EffortRawData!R$6</f>
         <v>44314</v>
       </c>
       <c r="B20" s="9">
         <f>EffortRawData!Q5</f>
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C20" s="9">
         <f t="shared" si="1"/>
@@ -4454,17 +4382,17 @@
       </c>
       <c r="D20" s="9">
         <f t="shared" si="2"/>
-        <v>55.5</v>
+        <v>12.25</v>
       </c>
       <c r="E20" s="2">
         <v>13</v>
       </c>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -4472,7 +4400,7 @@
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>

</xml_diff>